<commit_message>
updated rounded prism with extra explanatory column for rods disks
</commit_message>
<xml_diff>
--- a/raw_data/rounded prism_rods_disks.xlsx
+++ b/raw_data/rounded prism_rods_disks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhenders/Desktop/MgO_Ag_Project/Data Repo/pacigroup_nanocomposite_fem/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1DFF0D-4368-B441-B9E1-2E21519B7264}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708026B1-9F9B-BA4E-81D5-224696CFDD9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1160" windowWidth="27640" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Sx</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Applied Voltage and Results</t>
+  </si>
+  <si>
+    <t>Inclusion</t>
   </si>
 </sst>
 </file>
@@ -620,18 +623,18 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -987,905 +990,939 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB12"/>
+  <dimension ref="A1:AC12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:AB12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="6" t="s">
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="W2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="X2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="Y2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>223</v>
+      </c>
+      <c r="B3">
         <v>12.9872736</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>12.987171999999999</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>17.1742575</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1.72</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2.8588709670000001</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>2.9528627494999999</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>3.8675694319999998</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>7.5549867197770806E-2</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>7.5495804971126096E-2</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>60</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>160</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>9.26</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>1</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>0.5</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>50</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>64096</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="R3" s="1">
         <v>5.0000000000000003E-10</v>
       </c>
-      <c r="R3" s="1">
+      <c r="S3" s="1">
         <v>1.22328826632091E-15</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
         <v>2.9217592224306099E-15</v>
       </c>
-      <c r="T3" s="1">
+      <c r="U3" s="1">
         <v>4.2035156668298199E-14</v>
       </c>
-      <c r="U3" s="1">
+      <c r="V3" s="1">
         <v>4.6406684482768497E-18</v>
       </c>
-      <c r="V3" s="1">
+      <c r="W3" s="1">
         <v>7.8407884718105498E-11</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>14.4270115043233</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>0.5</v>
       </c>
-      <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>232</v>
+      </c>
+      <c r="B4">
         <v>12.9872736</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>17.1742575</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>12.987171999999999</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1.72</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2.8588709670000001</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>3.8675694319999998</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>2.9528627494999999</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>7.5549867197770695E-2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>7.5495427944766796E-2</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>60</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>160</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>9.26</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>1</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>0.5</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>50</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>63504</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="R4" s="1">
         <v>5.0000000000000003E-10</v>
       </c>
-      <c r="R4" s="1">
+      <c r="S4" s="1">
         <v>2.12517463838168E-15</v>
       </c>
-      <c r="S4" s="1">
+      <c r="T4" s="1">
         <v>4.7279854327951698E-15</v>
       </c>
-      <c r="T4" s="1">
+      <c r="U4" s="1">
         <v>6.6291394172795894E-14</v>
       </c>
-      <c r="U4" s="1">
+      <c r="V4" s="1">
         <v>7.3547921387429497E-18</v>
       </c>
-      <c r="V4" s="1">
+      <c r="W4" s="1">
         <v>1.34957090235789E-10</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>14.199909965727599</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>0.5</v>
       </c>
-      <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>17.194577890000001</v>
+        <v>332</v>
       </c>
       <c r="B5">
         <v>17.194577890000001</v>
       </c>
       <c r="C5">
+        <v>17.194577890000001</v>
+      </c>
+      <c r="D5">
         <v>13.144015830000001</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1.72</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>3.9296622695000001</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3.947494302</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>2.991499589</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>8.3079528645617004E-2</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>8.3033981390571998E-2</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>60</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>160</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>9.26</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>1</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>0.5</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>50</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>90993</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="R5" s="1">
         <v>5.0000000000000003E-10</v>
       </c>
-      <c r="R5" s="1">
+      <c r="S5" s="1">
         <v>1.9116000090363699E-15</v>
       </c>
-      <c r="S5" s="1">
+      <c r="T5" s="1">
         <v>4.7549564598370901E-15</v>
       </c>
-      <c r="T5" s="1">
+      <c r="U5" s="1">
         <v>6.9669534594847006E-14</v>
       </c>
-      <c r="U5" s="1">
+      <c r="V5" s="1">
         <v>7.2022719768170593E-18</v>
       </c>
-      <c r="V5" s="1">
+      <c r="W5" s="1">
         <v>1.7394221962224601E-10</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>13.974017924382499</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>0.5</v>
       </c>
-      <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>323</v>
+      </c>
+      <c r="B6">
         <v>17.194577890000001</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>13.144015830000001</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>17.194577890000001</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>1.72</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>3.9296622695000001</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>2.991499589</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>3.947494302</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>8.3079528645617004E-2</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>8.3034014972466694E-2</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>60</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>160</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>9.26</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>1</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>0.5</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>50</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>92597</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="R6" s="1">
         <v>5.0000000000000003E-10</v>
       </c>
-      <c r="R6" s="1">
+      <c r="S6" s="1">
         <v>1.1202806847106799E-15</v>
       </c>
-      <c r="S6" s="1">
+      <c r="T6" s="1">
         <v>2.71450914945391E-15</v>
       </c>
-      <c r="T6" s="1">
+      <c r="U6" s="1">
         <v>3.8096957276609799E-14</v>
       </c>
-      <c r="U6" s="1">
+      <c r="V6" s="1">
         <v>4.1074713006392399E-18</v>
       </c>
-      <c r="V6" s="1">
+      <c r="W6" s="1">
         <v>1.03734630562155E-10</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>14.261557049535901</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>0.5</v>
       </c>
-      <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>21.64774959</v>
+        <v>442</v>
       </c>
       <c r="B7">
         <v>21.64774959</v>
       </c>
       <c r="C7">
+        <v>21.64774959</v>
+      </c>
+      <c r="D7">
         <v>17.318199669999998</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1.72</v>
-      </c>
-      <c r="E7">
-        <v>5.0173155586932197</v>
       </c>
       <c r="F7">
         <v>5.0173155586932197</v>
       </c>
       <c r="G7">
+        <v>5.0173155586932197</v>
+      </c>
+      <c r="H7">
         <v>3.0721144534542502</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>6.8869981732813598E-2</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>6.8841737004298298E-2</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>60</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>160</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>9.26</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>1</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>0.5</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>50</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>123562</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="R7" s="1">
         <v>5.0000000000000003E-10</v>
       </c>
-      <c r="R7" s="1">
+      <c r="S7" s="1">
         <v>1.47043212286593E-15</v>
       </c>
-      <c r="S7" s="1">
+      <c r="T7" s="1">
         <v>3.19045302054705E-15</v>
       </c>
-      <c r="T7" s="1">
+      <c r="U7" s="1">
         <v>5.49113914020751E-14</v>
       </c>
-      <c r="U7" s="1">
+      <c r="V7" s="1">
         <v>4.2409104413917499E-18</v>
       </c>
-      <c r="V7" s="1">
+      <c r="W7" s="1">
         <v>1.8168953396555899E-10</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>12.133284883108001</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>0.5</v>
       </c>
-      <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>424</v>
+      </c>
+      <c r="B8">
         <v>21.64774959</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>17.318199669999998</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>21.64774959</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>1.72</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>5.0173155586932197</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>3.0721144534542502</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>5.0173155586932197</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>6.8869981732813598E-2</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>6.8841740537542898E-2</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>60</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>160</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>9.26</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>1</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>0.5</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>50</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>128461</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="R8" s="1">
         <v>5.0000000000000003E-10</v>
       </c>
-      <c r="R8" s="1">
+      <c r="S8" s="1">
         <v>9.7887865784770296E-16</v>
       </c>
-      <c r="S8" s="1">
+      <c r="T8" s="1">
         <v>1.7748993945266099E-15</v>
       </c>
-      <c r="T8" s="1">
+      <c r="U8" s="1">
         <v>2.2278640296692599E-14</v>
       </c>
-      <c r="U8" s="1">
+      <c r="V8" s="1">
         <v>2.0637156008547599E-18</v>
       </c>
-      <c r="V8" s="1">
+      <c r="W8" s="1">
         <v>1.25747731265773E-10</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>13.121052348061999</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>0.5</v>
       </c>
-      <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>12.93132224</v>
+        <v>224</v>
       </c>
       <c r="B9">
         <v>12.93132224</v>
       </c>
       <c r="C9">
+        <v>12.93132224</v>
+      </c>
+      <c r="D9">
         <v>17.241762990000002</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1.72</v>
-      </c>
-      <c r="E9">
-        <v>2.9436944011039698</v>
       </c>
       <c r="F9">
         <v>2.9436944011039698</v>
       </c>
       <c r="G9">
+        <v>2.9436944011039698</v>
+      </c>
+      <c r="H9">
         <v>4.8921377552124596</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.101001026368213</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.10094018282536101</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>60</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>160</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>9.26</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>1</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>0.5</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>50</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>72293</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="R9" s="1">
         <v>5.0000000000000003E-10</v>
       </c>
-      <c r="R9" s="1">
+      <c r="S9" s="1">
         <v>1.26422783092687E-15</v>
       </c>
-      <c r="S9" s="1">
+      <c r="T9" s="1">
         <v>3.0017923366769402E-15</v>
       </c>
-      <c r="T9" s="1">
+      <c r="U9" s="1">
         <v>4.1614102013056303E-14</v>
       </c>
-      <c r="U9" s="1">
+      <c r="V9" s="1">
         <v>6.1952306936642002E-18</v>
       </c>
-      <c r="V9" s="1">
+      <c r="W9" s="1">
         <v>9.1394822581196006E-11</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>17.0289805344526</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>0.5</v>
       </c>
-      <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>242</v>
+      </c>
+      <c r="B10">
         <v>12.93132224</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>17.241762990000002</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>12.93132224</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>1.72</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>2.9436944011039698</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>4.8921377552124596</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>2.9436944011039698</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.101001026368213</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.100940169893961</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>60</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>160</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>9.26</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>1</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>0.5</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>50</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>69645</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="R10" s="1">
         <v>5.0000000000000003E-10</v>
       </c>
-      <c r="R10" s="1">
+      <c r="S10" s="1">
         <v>2.0821124784567701E-15</v>
       </c>
-      <c r="S10" s="1">
+      <c r="T10" s="1">
         <v>4.9816713355500397E-15</v>
       </c>
-      <c r="T10" s="1">
+      <c r="U10" s="1">
         <v>7.4444126618106003E-14</v>
       </c>
-      <c r="U10" s="1">
+      <c r="V10" s="1">
         <v>8.2182099291462496E-18</v>
       </c>
-      <c r="V10" s="1">
+      <c r="W10" s="1">
         <v>1.4500872356212301E-10</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>15.1979045020915</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>0.5</v>
       </c>
-      <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>12.93132224</v>
+        <v>225</v>
       </c>
       <c r="B11">
         <v>12.93132224</v>
       </c>
       <c r="C11">
+        <v>12.93132224</v>
+      </c>
+      <c r="D11">
         <v>21.552203739999999</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1.72</v>
-      </c>
-      <c r="E11">
-        <v>2.9682516569585502</v>
       </c>
       <c r="F11">
         <v>2.9682516569585502</v>
       </c>
       <c r="G11">
+        <v>2.9682516569585502</v>
+      </c>
+      <c r="H11">
         <v>5.9152985092756296</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0.100876756578203</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.100821584715101</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>60</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>160</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>9.26</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>1</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>0.5</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>50</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>90047</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="R11" s="1">
         <v>5.0000000000000003E-10</v>
       </c>
-      <c r="R11" s="1">
+      <c r="S11" s="1">
         <v>7.88752971821596E-16</v>
       </c>
-      <c r="S11" s="1">
+      <c r="T11" s="1">
         <v>1.97954185986048E-15</v>
       </c>
-      <c r="T11" s="1">
+      <c r="U11" s="1">
         <v>3.9657722093949299E-14</v>
       </c>
-      <c r="U11" s="1">
+      <c r="V11" s="1">
         <v>2.8305388367745602E-18</v>
       </c>
-      <c r="V11" s="1">
+      <c r="W11" s="1">
         <v>7.10248388536193E-11</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>16.5419736627682</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>0.5</v>
       </c>
-      <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>252</v>
+      </c>
+      <c r="B12">
         <v>12.93132224</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>21.552203739999999</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>12.93132224</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1.72</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>2.9682516569585502</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>5.9152985092756296</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>2.9682516569585502</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.100876756578203</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.100821845442276</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>60</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>160</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>9.26</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>1</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>0.5</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>50</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>89358</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="R12" s="1">
         <v>5.0000000000000003E-10</v>
       </c>
-      <c r="R12" s="1">
+      <c r="S12" s="1">
         <v>1.9867468038516599E-15</v>
       </c>
-      <c r="S12" s="1">
+      <c r="T12" s="1">
         <v>4.7379214750233101E-15</v>
       </c>
-      <c r="T12" s="1">
+      <c r="U12" s="1">
         <v>6.1422590824851396E-14</v>
       </c>
-      <c r="U12" s="1">
+      <c r="V12" s="1">
         <v>8.5460945850628806E-18</v>
       </c>
-      <c r="V12" s="1">
+      <c r="W12" s="1">
         <v>1.7753172089857699E-10</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>14.885229377746599</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <v>0.5</v>
       </c>
-      <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="O1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>